<commit_message>
1.Small update to registers spreadsheet. 2. Adding channel map text file for convenient look up. This maps index in received snapshots to index of ADC output stream and vice versa. 3.Latest versions of several tests in notebooks.
</commit_message>
<xml_diff>
--- a/cosmic_ray_scripts/snap2_control/cr_registers.xlsx
+++ b/cosmic_ray_scripts/snap2_control/cr_registers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4566bfd2e2f5f505/Documents/research/LWA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="139" documentId="14_{42B3502A-86A0-45ED-BFF9-DC592E8603F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F62F8D53-056E-4F8F-9F29-84F58FE29A3D}"/>
+  <xr:revisionPtr revIDLastSave="157" documentId="14_{42B3502A-86A0-45ED-BFF9-DC592E8603F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{722F53E2-942F-43FF-B8F1-71CC9A283609}"/>
   <bookViews>
-    <workbookView xWindow="4410" yWindow="2355" windowWidth="16905" windowHeight="11040" xr2:uid="{028AD5E7-3E96-4DE2-B0D1-9553BB825CBB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{028AD5E7-3E96-4DE2-B0D1-9553BB825CBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="104">
   <si>
     <t>bitwidth</t>
   </si>
@@ -340,6 +340,12 @@
   </si>
   <si>
     <t>cosmic_ray_wait_between_packets</t>
+  </si>
+  <si>
+    <t>brd_id</t>
+  </si>
+  <si>
+    <t>Number to identify each SNAP2 board</t>
   </si>
 </sst>
 </file>
@@ -691,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{663B0E9B-1259-49B3-93EE-CE90EC2AA12E}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1283,10 +1289,10 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="B26">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C26" t="s">
         <v>79</v>
@@ -1301,35 +1307,35 @@
         <v>17</v>
       </c>
       <c r="G26" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="D27">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="E27">
         <v>32</v>
       </c>
       <c r="F27" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G27" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -1338,7 +1344,7 @@
         <v>56</v>
       </c>
       <c r="D28">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E28">
         <v>32</v>
@@ -1347,21 +1353,21 @@
         <v>16</v>
       </c>
       <c r="G28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B29">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E29">
         <v>32</v>
@@ -1370,18 +1376,18 @@
         <v>16</v>
       </c>
       <c r="G29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B30">
         <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -1393,18 +1399,18 @@
         <v>16</v>
       </c>
       <c r="G30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B31">
         <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -1416,18 +1422,18 @@
         <v>16</v>
       </c>
       <c r="G31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B32">
         <v>32</v>
       </c>
       <c r="C32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -1439,18 +1445,18 @@
         <v>16</v>
       </c>
       <c r="G32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B33">
         <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1462,18 +1468,18 @@
         <v>16</v>
       </c>
       <c r="G33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="B34">
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -1485,18 +1491,18 @@
         <v>16</v>
       </c>
       <c r="G34" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B35">
         <v>32</v>
       </c>
       <c r="C35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -1508,18 +1514,18 @@
         <v>16</v>
       </c>
       <c r="G35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B36">
         <v>32</v>
       </c>
       <c r="C36" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -1531,29 +1537,52 @@
         <v>16</v>
       </c>
       <c r="G36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="C37" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D37">
         <v>0</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="F37" t="s">
         <v>16</v>
       </c>
       <c r="G37" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>99</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
+        <v>16</v>
+      </c>
+      <c r="G38" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding new trigger counter to register spreadsheet
</commit_message>
<xml_diff>
--- a/cosmic_ray_scripts/snap2_control/cr_registers.xlsx
+++ b/cosmic_ray_scripts/snap2_control/cr_registers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4566bfd2e2f5f505/Documents/research/LWA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="157" documentId="14_{42B3502A-86A0-45ED-BFF9-DC592E8603F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{722F53E2-942F-43FF-B8F1-71CC9A283609}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{361C9EEE-8C57-47C1-9A4B-D88DE4A9EC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{028AD5E7-3E96-4DE2-B0D1-9553BB825CBB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{028AD5E7-3E96-4DE2-B0D1-9553BB825CBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="107">
   <si>
     <t>bitwidth</t>
   </si>
@@ -346,14 +346,31 @@
   </si>
   <si>
     <t>Number to identify each SNAP2 board</t>
+  </si>
+  <si>
+    <t>internal_trigger_count</t>
+  </si>
+  <si>
+    <t>cosmic_ray_internal_trigger_count</t>
+  </si>
+  <si>
+    <t>Counts the number of triggers output by the coincidence_trigger block. These are the internally generated triggers that made it past the veto.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -381,8 +398,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -697,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{663B0E9B-1259-49B3-93EE-CE90EC2AA12E}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,26 +730,26 @@
     <col min="6" max="6" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1586,7 +1604,31 @@
         <v>98</v>
       </c>
     </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>104</v>
+      </c>
+      <c r="B39">
+        <v>32</v>
+      </c>
+      <c r="C39" t="s">
+        <v>105</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>32</v>
+      </c>
+      <c r="F39" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39" t="s">
+        <v>106</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>